<commit_message>
Some Question of Strings
</commit_message>
<xml_diff>
--- a/DSA by Shradha Didi & Aman Bhaiya.xlsx
+++ b/DSA by Shradha Didi & Aman Bhaiya.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MY_STUDY_SPACE\DSA 375\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MY_STUDY_SPACE\DSA 375\DSA_375\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7789567-9C4B-4FFC-8B64-ED1285138FA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB146B63-E573-4CF1-8DBA-DF8A25BDD87B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1241" uniqueCount="700">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1257" uniqueCount="701">
   <si>
     <t>DSA by Shradha Didi &amp; Aman Bhaiya</t>
   </si>
@@ -2149,6 +2149,9 @@
   </si>
   <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t>DOne</t>
   </si>
 </sst>
 </file>
@@ -2733,8 +2736,8 @@
   </sheetPr>
   <dimension ref="A1:Z919"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="C32" workbookViewId="0">
+      <selection activeCell="J46" sqref="J46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3281,7 +3284,9 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
+      <c r="J17" s="2" t="s">
+        <v>699</v>
+      </c>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
@@ -3315,7 +3320,9 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
+      <c r="J18" s="2" t="s">
+        <v>700</v>
+      </c>
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
@@ -3349,7 +3356,9 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
+      <c r="J19" s="2" t="s">
+        <v>699</v>
+      </c>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
@@ -3383,7 +3392,9 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
+      <c r="J20" s="2" t="s">
+        <v>699</v>
+      </c>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
@@ -3417,7 +3428,9 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
+      <c r="J21" s="2" t="s">
+        <v>699</v>
+      </c>
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
@@ -3453,7 +3466,9 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
+      <c r="J22" s="2" t="s">
+        <v>699</v>
+      </c>
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
@@ -3487,7 +3502,9 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
+      <c r="J23" s="2" t="s">
+        <v>699</v>
+      </c>
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
@@ -3521,7 +3538,9 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
+      <c r="J24" s="2" t="s">
+        <v>699</v>
+      </c>
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
@@ -3555,7 +3574,9 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
+      <c r="J25" s="2" t="s">
+        <v>699</v>
+      </c>
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
@@ -4055,7 +4076,9 @@
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
-      <c r="J40" s="2"/>
+      <c r="J40" s="2" t="s">
+        <v>699</v>
+      </c>
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
       <c r="M40" s="2"/>
@@ -4089,7 +4112,9 @@
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
-      <c r="J41" s="2"/>
+      <c r="J41" s="2" t="s">
+        <v>699</v>
+      </c>
       <c r="K41" s="2"/>
       <c r="L41" s="2"/>
       <c r="M41" s="2"/>
@@ -4125,7 +4150,9 @@
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
-      <c r="J42" s="2"/>
+      <c r="J42" s="2" t="s">
+        <v>699</v>
+      </c>
       <c r="K42" s="2"/>
       <c r="L42" s="2"/>
       <c r="M42" s="2"/>
@@ -4159,7 +4186,9 @@
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
-      <c r="J43" s="2"/>
+      <c r="J43" s="2" t="s">
+        <v>699</v>
+      </c>
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
       <c r="M43" s="2"/>
@@ -4193,7 +4222,9 @@
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
-      <c r="J44" s="2"/>
+      <c r="J44" s="2" t="s">
+        <v>699</v>
+      </c>
       <c r="K44" s="2"/>
       <c r="L44" s="2"/>
       <c r="M44" s="2"/>
@@ -4227,7 +4258,9 @@
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
       <c r="I45" s="2"/>
-      <c r="J45" s="2"/>
+      <c r="J45" s="2" t="s">
+        <v>699</v>
+      </c>
       <c r="K45" s="2"/>
       <c r="L45" s="2"/>
       <c r="M45" s="2"/>
@@ -4261,7 +4294,9 @@
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
       <c r="I46" s="2"/>
-      <c r="J46" s="2"/>
+      <c r="J46" s="2" t="s">
+        <v>699</v>
+      </c>
       <c r="K46" s="2"/>
       <c r="L46" s="2"/>
       <c r="M46" s="2"/>
@@ -30613,19 +30648,19 @@
   <customSheetViews>
     <customSheetView guid="{CA88BB58-64FD-4028-BB60-AD1F55D0D3FB}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:C37" xr:uid="{3759BBE4-7A0E-4F85-85AD-CB3100E413B3}"/>
+      <autoFilter ref="A11:C37" xr:uid="{99988A40-8C23-4CF5-8CC3-A9ADB05B4A2D}"/>
     </customSheetView>
     <customSheetView guid="{9692B2DD-7D60-44BD-B856-1EB36C066BC2}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:D37" xr:uid="{0AD9A8F7-1FBD-4B7D-B9A9-00DD4625C064}"/>
+      <autoFilter ref="A11:D37" xr:uid="{2A0E6E5D-A174-48AE-AE56-CD8067A565F6}"/>
     </customSheetView>
     <customSheetView guid="{56F64459-0E4A-49E2-8D3D-866C350B0872}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:D37" xr:uid="{71549760-442A-48E2-B44D-63CA3F55310C}"/>
+      <autoFilter ref="A11:D37" xr:uid="{A8987AFC-90E4-44EB-BED3-6C487EC8248D}"/>
     </customSheetView>
     <customSheetView guid="{DFF38759-4F02-4A18-8E61-B0B0F994C4E2}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A293:C332" xr:uid="{4BDF63E0-EF9B-4CDB-9238-603FBBD506CE}"/>
+      <autoFilter ref="A293:C332" xr:uid="{AE58965C-6B6B-4CDD-89FC-D8F3945EBC6B}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="3">
@@ -31034,14 +31069,14 @@
     <col min="3" max="3" width="38.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="24.6" x14ac:dyDescent="0.25">
       <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="40"/>
       <c r="C1" s="40"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="41" t="s">
         <v>1</v>
       </c>
@@ -31117,7 +31152,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
         <v>128</v>
       </c>
@@ -31125,7 +31160,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
         <v>128</v>
       </c>
@@ -31133,7 +31168,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
         <v>128</v>
       </c>
@@ -31141,7 +31176,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
         <v>128</v>
       </c>
@@ -31149,7 +31184,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A19" s="24" t="s">
         <v>128</v>
       </c>
@@ -31157,7 +31192,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A20" s="24" t="s">
         <v>128</v>
       </c>
@@ -31165,7 +31200,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A21" s="24" t="s">
         <v>128</v>
       </c>

</xml_diff>